<commit_message>
fix : CU-SAS002 BOM
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/CU-SAS002.xlsx
+++ b/機械設計/_BOM/CU-SAS002.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C51D8E27-CB44-43AA-A08C-869AFC9B5AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF7B301C-603F-47FF-9353-72384A9FB777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17970" yWindow="-2220" windowWidth="14400" windowHeight="10845" xr2:uid="{9169827C-64E3-473A-8865-40248F252642}"/>
+    <workbookView xWindow="-17970" yWindow="-2220" windowWidth="14400" windowHeight="10845" xr2:uid="{A6ED1731-D352-42D6-8412-CD520A5842D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{353BE805-F0AD-4590-8F99-907197396DE2}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="-148" windowWidth="960" windowHeight="723" activeSheetId="1"/>
+    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{25495C1B-1C95-4E03-95F2-0C114AEACF78}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="-148" windowWidth="960" windowHeight="723" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="77">
   <si>
     <t>種類</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>無</t>
-  </si>
-  <si>
-    <t>CU-SAS</t>
   </si>
   <si>
     <t>CU-AAS-P002</t>
@@ -356,8 +353,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{82AD201C-3F09-4D38-88B6-4BB3F9C43F4F}">
-  <header guid="{82AD201C-3F09-4D38-88B6-4BB3F9C43F4F}" dateTime="2023-07-13T16:13:16" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{EBAC2BC7-F2AC-4EE4-BD82-44FE2470FE13}">
+  <header guid="{EBAC2BC7-F2AC-4EE4-BD82-44FE2470FE13}" dateTime="2023-07-13T16:22:57" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -669,7 +666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059275E-F0FA-4410-8824-8206E0F32B16}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C24A8B-C2F2-4A37-B4CC-481BCA4AE1E9}">
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -798,15 +795,15 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>22</v>
@@ -837,18 +834,18 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -864,19 +861,19 @@
         <v>23</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -884,18 +881,18 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
@@ -911,19 +908,19 @@
         <v>23</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -931,18 +928,18 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -958,19 +955,19 @@
         <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -978,17 +975,17 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>22</v>
@@ -1001,10 +998,10 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="M7" s="3">
         <v>580</v>
@@ -1022,18 +1019,18 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
@@ -1044,7 +1041,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="3"/>
@@ -1061,19 +1058,19 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
@@ -1081,10 +1078,10 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="3">
         <v>260</v>
@@ -1102,21 +1099,21 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -1124,7 +1121,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="3"/>
@@ -1132,36 +1129,36 @@
         <v>23</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -1169,10 +1166,10 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="3">
         <v>330</v>
@@ -1190,19 +1187,19 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H12" s="1">
         <v>3</v>
@@ -1210,10 +1207,10 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="M12" s="3">
         <v>510</v>
@@ -1231,19 +1228,19 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H13" s="1">
         <v>4</v>
@@ -1251,10 +1248,10 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M13" s="3">
         <v>280</v>
@@ -1272,19 +1269,19 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H14" s="1">
         <v>8</v>
@@ -1292,10 +1289,10 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M14" s="3">
         <v>280</v>
@@ -1313,18 +1310,18 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1">
@@ -1332,7 +1329,7 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1346,17 +1343,17 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H16" s="1">
         <v>6</v>
@@ -1375,18 +1372,18 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>22</v>
@@ -1414,18 +1411,18 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
@@ -1437,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1455,18 +1452,18 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>22</v>
@@ -1494,18 +1491,18 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>22</v>
@@ -1517,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1535,18 +1532,18 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>22</v>
@@ -1558,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1576,7 +1573,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{353BE805-F0AD-4590-8F99-907197396DE2}">
+    <customSheetView guid="{25495C1B-1C95-4E03-95F2-0C114AEACF78}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
     </customSheetView>

</xml_diff>